<commit_message>
xcelUtils implementation phase 2 (excel file)
</commit_message>
<xml_diff>
--- a/src/test/resources/Datasheet.xlsx
+++ b/src/test/resources/Datasheet.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2481C1-B97A-4B05-B4E0-EFE9DCB35380}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>firstname</t>
   </si>
@@ -27,27 +28,6 @@
     <t>lastname</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>bookingid</t>
-  </si>
-  <si>
-    <t>roomid</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>Jean</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>jean.doe@jeandoe.com</t>
-  </si>
-  <si>
     <t>2020-03-19</t>
   </si>
   <si>
@@ -61,12 +41,27 @@
   </si>
   <si>
     <t>depositpaid</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Adjei</t>
+  </si>
+  <si>
+    <t>totalprice</t>
+  </si>
+  <si>
+    <t>additionalneeds</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,27 +415,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -448,10 +441,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -460,47 +453,35 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>500</v>
+      </c>
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1">
-        <v>101</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2255</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1234678998234340</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" display="carlos@adj" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
xcelUtils implementation phase 3 (excel file)
</commit_message>
<xml_diff>
--- a/src/test/resources/Datasheet.xlsx
+++ b/src/test/resources/Datasheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2481C1-B97A-4B05-B4E0-EFE9DCB35380}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D673C0E-905C-4B11-A0E1-162FD02A42DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,10 +427,10 @@
     <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>